<commit_message>
update generate_story với việc thêm cột "week" vào work.
update generate_story với việc thêm cột "week" vào work. (Trước đó bị bug vì thêm cột "week" vào có vẻ làm hỏng định dạng file của data.xlsx -> generate_story bị bug (trong khi generate_ipa và generate_meaning không bị).
</commit_message>
<xml_diff>
--- a/deploy/backend/uploads/data.xlsx
+++ b/deploy/backend/uploads/data.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/GIT/MiniProd_ContentEngFlow_IELTSStepUpE_T102024/deploy/backend/uploads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_690C9FCDAE3DB4E6AB6EC90AFCAE670FAE24A5A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8B2E838-37BB-4A8C-8A77-ECB961B60FE9}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>order</t>
   </si>
@@ -26,9 +43,6 @@
   </si>
   <si>
     <t>MAIN QUESTION</t>
-  </si>
-  <si>
-    <t>set</t>
   </si>
   <si>
     <t>vocabulary</t>
@@ -111,24 +125,6 @@
     <t xml:space="preserve">,"voice": "en-CA-ClaraNeural","speed": 1}' --output </t>
   </si>
   <si>
-    <t>You are now a award-winning writer. You write  conversations between a man an a woman.
-- Language: Vietnamese. Setting: in the western countries.
-- use American names for 2 people.
-- Anh/chị - em, cậu - tớ, bố/mẹ - con correspoding relationship between them.
-- The conversation will have 2 turns, each person talk twice
-- The conversation is intersting, dramatic, witty, humourous, and natural. 
-- the content doesn't have &lt;r&gt; tag
-- The translation_en contain the given vocab in  &lt;r&gt; vocab &lt;/r&gt;
-- The given word appear only once in translation_en.
-- &lt;gender&gt; are exactly 'male' and 'female'
-EXAMPLE:
-go to school - đi học:
-"content":"Tớ muốn đi học cơ" 
-"translation_en":"I really want to &lt;r&gt;go to school&lt;/r&gt;!"
-output format:
-[{"situation":"brief desctiption of 2 people name, their relation, where they are","situation_en":"translate situation to English","conversation":[{"role":"&lt;gender&gt;_1","content":"their dialog","translation_en":"English translation"},{"role":"&lt;other_gender&gt;_1","content":"their dialog","translation_en":"English translation"},{"role":"&lt;gender&gt;_2","content":"their dialog","translation_en":"English translation"},{"role":"&lt;other_gender&gt;_2","content":"their dialog","translation_en":"English translation"}]}]</t>
-  </si>
-  <si>
     <t>Generational family</t>
   </si>
   <si>
@@ -137,14 +133,19 @@
   <si>
     <t>Topic: Family size and type
 Vocab: Generational family</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>set</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,7 +155,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -166,7 +173,7 @@
     </font>
     <font>
       <sz val="24"/>
-      <color rgb="FF2d2e2d"/>
+      <color rgb="FF2D2E2D"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -203,16 +210,16 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </right>
       <top style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFcccccc"/>
+        <color rgb="FFCCCCCC"/>
       </bottom>
       <diagonal/>
     </border>
@@ -220,47 +227,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -271,10 +296,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -312,71 +337,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,7 +429,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -427,11 +452,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -440,13 +465,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -456,7 +481,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -465,7 +490,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -474,7 +499,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -482,10 +507,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -550,219 +575,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="9" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="26.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="55.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="34.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="60.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="9.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33.75" customFormat="1" s="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="16">
         <v>10</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="B2" s="6">
+        <v>3000</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="str">
+        <f>"Topic: "&amp;E2&amp;" - "&amp;F2&amp;CHAR(10)&amp;"Given vocabulary: "&amp;G2&amp;CHAR(10)&amp;"Situation: "&amp;H2</f>
+        <v>Topic: talk about your family - Family size and type
+Given vocabulary: Nuclear family
+Situation: Sarah and Tom, neighbors, at a community park</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="10" t="str">
+        <f>O2&amp;""""&amp;G2&amp;""""&amp;P2&amp;B2&amp;"/ipa.mp3"</f>
+        <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Nuclear family","voice": "en-CA-ClaraNeural","speed": 1}' --output 3000/ipa.mp3</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="2241.75" customFormat="1" s="1">
-      <c r="A2" s="4">
-        <v>999</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:17" ht="409.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7" t="str">
+        <f>"Topic: "&amp;E3&amp;" - "&amp;F3&amp;CHAR(10)&amp;"Given vocabulary: "&amp;G3&amp;CHAR(10)&amp;"Situation: "&amp;H3</f>
+        <v>Topic: talk about your family - Family size and type
+Given vocabulary: Generational family
+Situation: Aubrey and Isaac, engineers, at a construction site</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5">
-        <f>"Topic: "&amp;D2&amp;" - "&amp;E2&amp;char(10)&amp;"Given vocabulary: "&amp;F2&amp;char(10)&amp;"Situation: "&amp;G2</f>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="L3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="3" t="s">
+      <c r="P3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="5">
-        <f>N2&amp;""&amp;G2&amp;"""&amp;O2&amp;A2&amp;"/ipa.mp3"</f>
+      <c r="Q3" s="12" t="str">
+        <f>O3&amp;""""&amp;G3&amp;""""&amp;P3&amp;B3&amp;"/ipa.MP4"</f>
+        <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Generational family","voice": "en-CA-ClaraNeural","speed": 1}' --output 2000/ipa.MP4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="2193" customFormat="1" s="1">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5">
-        <f>"Topic: "&amp;D3&amp;" - "&amp;E3&amp;char(10)&amp;"Given vocabulary: "&amp;F3&amp;char(10)&amp;"Situation: "&amp;G3</f>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="5">
-        <f>N3&amp;""&amp;G3&amp;"""&amp;O3&amp;A3&amp;"/ipa.MP4"</f>
-      </c>
+    <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+    <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>